<commit_message>
Raporum and Tablolarım are done
</commit_message>
<xml_diff>
--- a/yapay_bilanco_2020_2024.xlsx
+++ b/yapay_bilanco_2020_2024.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ugurc\Desktop\financial_dashboard\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>A Hazır Değerler</t>
   </si>
@@ -125,13 +130,16 @@
   </si>
   <si>
     <t>Toplam Pasif</t>
+  </si>
+  <si>
+    <t>Yıllar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,10 +191,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -194,6 +205,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -240,7 +259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,9 +291,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,6 +326,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -481,14 +502,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,7 +625,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2020</v>
       </c>
@@ -654,58 +678,58 @@
         <v>99663</v>
       </c>
       <c r="R2">
-        <v>47446.49750833215</v>
+        <v>47446.497508332148</v>
       </c>
       <c r="S2">
-        <v>68751.25989398666</v>
+        <v>68751.259893986658</v>
       </c>
       <c r="T2">
-        <v>71868.62891877038</v>
+        <v>71868.628918770381</v>
       </c>
       <c r="U2">
         <v>51860.61687349312</v>
       </c>
       <c r="V2">
-        <v>56821.3133748759</v>
+        <v>56821.313374875899</v>
       </c>
       <c r="W2">
-        <v>34849.38233583888</v>
+        <v>34849.382335838884</v>
       </c>
       <c r="X2">
-        <v>34188.47817685435</v>
+        <v>34188.478176854347</v>
       </c>
       <c r="Y2">
-        <v>21661.05550453836</v>
+        <v>21661.055504538359</v>
       </c>
       <c r="Z2">
-        <v>73713.52251896894</v>
+        <v>73713.522518968937</v>
       </c>
       <c r="AA2">
-        <v>53510.52808555523</v>
+        <v>53510.528085555226</v>
       </c>
       <c r="AB2">
-        <v>66019.15727467735</v>
+        <v>66019.157274677345</v>
       </c>
       <c r="AC2">
-        <v>75159.83766309742</v>
+        <v>75159.837663097424</v>
       </c>
       <c r="AD2">
-        <v>43566.42629059708</v>
+        <v>43566.426290597083</v>
       </c>
       <c r="AE2">
-        <v>66839.02297901007</v>
+        <v>66839.022979010071</v>
       </c>
       <c r="AF2">
-        <v>47625.81866047369</v>
+        <v>47625.818660473691</v>
       </c>
       <c r="AG2">
-        <v>21376.80407123103</v>
+        <v>21376.804071231029</v>
       </c>
       <c r="AH2">
-        <v>6024.094425436108</v>
+        <v>6024.0944254361084</v>
       </c>
       <c r="AI2">
-        <v>21012.68033434974</v>
+        <v>21012.680334349741</v>
       </c>
       <c r="AJ2">
         <v>21123.87510991349</v>
@@ -714,10 +738,10 @@
         <v>883419</v>
       </c>
       <c r="AL2">
-        <v>883418.9999999999</v>
+        <v>883418.99999999988</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2021</v>
       </c>
@@ -773,58 +797,58 @@
         <v>101718.1104824995</v>
       </c>
       <c r="S3">
-        <v>15307.28178252017</v>
+        <v>15307.281782520169</v>
       </c>
       <c r="T3">
-        <v>47311.17320769253</v>
+        <v>47311.173207692533</v>
       </c>
       <c r="U3">
-        <v>57916.19706669252</v>
+        <v>57916.197066692519</v>
       </c>
       <c r="V3">
-        <v>8255.504157309553</v>
+        <v>8255.5041573095532</v>
       </c>
       <c r="W3">
-        <v>40938.50333187462</v>
+        <v>40938.503331874621</v>
       </c>
       <c r="X3">
-        <v>9184.583637521388</v>
+        <v>9184.5836375213876</v>
       </c>
       <c r="Y3">
         <v>14367.47390184399</v>
       </c>
       <c r="Z3">
-        <v>43151.77234766795</v>
+        <v>43151.772347667953</v>
       </c>
       <c r="AA3">
-        <v>17127.89134131865</v>
+        <v>17127.891341318649</v>
       </c>
       <c r="AB3">
-        <v>34616.25693823912</v>
+        <v>34616.256938239123</v>
       </c>
       <c r="AC3">
-        <v>5585.205281735352</v>
+        <v>5585.2052817353524</v>
       </c>
       <c r="AD3">
         <v>59022.29515456596</v>
       </c>
       <c r="AE3">
-        <v>82512.12797123817</v>
+        <v>82512.127971238166</v>
       </c>
       <c r="AF3">
-        <v>72548.66246000571</v>
+        <v>72548.662460005711</v>
       </c>
       <c r="AG3">
-        <v>52123.9336559954</v>
+        <v>52123.933655995403</v>
       </c>
       <c r="AH3">
-        <v>79565.036363684</v>
+        <v>79565.036363684005</v>
       </c>
       <c r="AI3">
-        <v>24725.74455016417</v>
+        <v>24725.744550164171</v>
       </c>
       <c r="AJ3">
-        <v>52850.24636743122</v>
+        <v>52850.246367431217</v>
       </c>
       <c r="AK3">
         <v>818828</v>
@@ -833,7 +857,7 @@
         <v>818828</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2022</v>
       </c>
@@ -886,13 +910,13 @@
         <v>96387</v>
       </c>
       <c r="R4">
-        <v>35988.38581772489</v>
+        <v>35988.385817724891</v>
       </c>
       <c r="S4">
         <v>116967.6686645615</v>
       </c>
       <c r="T4">
-        <v>17290.27450463216</v>
+        <v>17290.274504632162</v>
       </c>
       <c r="U4">
         <v>58318.84350269194</v>
@@ -901,13 +925,13 @@
         <v>67767.27587512965</v>
       </c>
       <c r="W4">
-        <v>24189.31189631907</v>
+        <v>24189.311896319068</v>
       </c>
       <c r="X4">
-        <v>40583.92189746907</v>
+        <v>40583.921897469067</v>
       </c>
       <c r="Y4">
-        <v>45273.738451264</v>
+        <v>45273.738451263998</v>
       </c>
       <c r="Z4">
         <v>104948.1822835506</v>
@@ -916,31 +940,31 @@
         <v>37633.1978717725</v>
       </c>
       <c r="AB4">
-        <v>73885.31420474748</v>
+        <v>73885.314204747483</v>
       </c>
       <c r="AC4">
-        <v>117282.3615982174</v>
+        <v>117282.36159821739</v>
       </c>
       <c r="AD4">
         <v>75511.0153518929</v>
       </c>
       <c r="AE4">
-        <v>77773.74672911099</v>
+        <v>77773.746729110993</v>
       </c>
       <c r="AF4">
         <v>110504.3599502443</v>
       </c>
       <c r="AG4">
-        <v>87966.23041027357</v>
+        <v>87966.230410273565</v>
       </c>
       <c r="AH4">
         <v>39418.1565764361</v>
       </c>
       <c r="AI4">
-        <v>39629.65061282022</v>
+        <v>39629.650612820224</v>
       </c>
       <c r="AJ4">
-        <v>36662.36380114176</v>
+        <v>36662.363801141757</v>
       </c>
       <c r="AK4">
         <v>1207594</v>
@@ -949,7 +973,7 @@
         <v>1207594</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2023</v>
       </c>
@@ -1002,61 +1026,61 @@
         <v>6016</v>
       </c>
       <c r="R5">
-        <v>21797.22080787508</v>
+        <v>21797.220807875081</v>
       </c>
       <c r="S5">
         <v>12784.47916666667</v>
       </c>
       <c r="T5">
-        <v>32021.82841140529</v>
+        <v>32021.828411405291</v>
       </c>
       <c r="U5">
-        <v>5630.080787508486</v>
+        <v>5630.0807875084856</v>
       </c>
       <c r="V5">
-        <v>7631.259080108622</v>
+        <v>7631.2590801086217</v>
       </c>
       <c r="W5">
-        <v>49737.83579429735</v>
+        <v>49737.835794297353</v>
       </c>
       <c r="X5">
-        <v>51707.02499151391</v>
+        <v>51707.024991513907</v>
       </c>
       <c r="Y5">
-        <v>62194.9846826205</v>
+        <v>62194.984682620503</v>
       </c>
       <c r="Z5">
-        <v>62918.08702477936</v>
+        <v>62918.087024779357</v>
       </c>
       <c r="AA5">
-        <v>56235.34181941616</v>
+        <v>56235.341819416157</v>
       </c>
       <c r="AB5">
-        <v>65427.37118126272</v>
+        <v>65427.371181262723</v>
       </c>
       <c r="AC5">
-        <v>69109.09288017651</v>
+        <v>69109.092880176511</v>
       </c>
       <c r="AD5">
-        <v>69140.3380431093</v>
+        <v>69140.338043109296</v>
       </c>
       <c r="AE5">
-        <v>53722.33800067888</v>
+        <v>53722.338000678879</v>
       </c>
       <c r="AF5">
-        <v>59849.36566530889</v>
+        <v>59849.365665308891</v>
       </c>
       <c r="AG5">
-        <v>35379.19556177868</v>
+        <v>35379.195561778681</v>
       </c>
       <c r="AH5">
-        <v>40116.5574083503</v>
+        <v>40116.557408350302</v>
       </c>
       <c r="AI5">
-        <v>60084.4483197556</v>
+        <v>60084.448319755596</v>
       </c>
       <c r="AJ5">
-        <v>26097.15037338764</v>
+        <v>26097.150373387642</v>
       </c>
       <c r="AK5">
         <v>841584</v>
@@ -1065,7 +1089,7 @@
         <v>841584</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2024</v>
       </c>
@@ -1118,67 +1142,67 @@
         <v>94789</v>
       </c>
       <c r="R6">
-        <v>63088.75559164873</v>
+        <v>63088.755591648733</v>
       </c>
       <c r="S6">
-        <v>54821.34780457389</v>
+        <v>54821.347804573888</v>
       </c>
       <c r="T6">
-        <v>44855.13573425589</v>
+        <v>44855.135734255891</v>
       </c>
       <c r="U6">
-        <v>53934.04373554318</v>
+        <v>53934.043735543179</v>
       </c>
       <c r="V6">
-        <v>73839.33807550737</v>
+        <v>73839.338075507374</v>
       </c>
       <c r="W6">
         <v>14096.32525494298</v>
       </c>
       <c r="X6">
-        <v>45682.59465474587</v>
+        <v>45682.594654745873</v>
       </c>
       <c r="Y6">
-        <v>45686.58433131524</v>
+        <v>45686.584331315244</v>
       </c>
       <c r="Z6">
-        <v>71535.6988243458</v>
+        <v>71535.698824345804</v>
       </c>
       <c r="AA6">
-        <v>10460.93196492146</v>
+        <v>10460.931964921459</v>
       </c>
       <c r="AB6">
-        <v>9503.409588269606</v>
+        <v>9503.4095882696056</v>
       </c>
       <c r="AC6">
-        <v>22676.52368505743</v>
+        <v>22676.523685057429</v>
       </c>
       <c r="AD6">
-        <v>18465.02109841704</v>
+        <v>18465.021098417041</v>
       </c>
       <c r="AE6">
-        <v>30981.43443188447</v>
+        <v>30981.434431884471</v>
       </c>
       <c r="AF6">
-        <v>78537.58120361246</v>
+        <v>78537.581203612455</v>
       </c>
       <c r="AG6">
-        <v>43152.34177444335</v>
+        <v>43152.341774443346</v>
       </c>
       <c r="AH6">
-        <v>38253.81688255526</v>
+        <v>38253.816882555257</v>
       </c>
       <c r="AI6">
-        <v>16522.84654444154</v>
+        <v>16522.846544441541</v>
       </c>
       <c r="AJ6">
-        <v>57325.26881951847</v>
+        <v>57325.268819518467</v>
       </c>
       <c r="AK6">
         <v>793419</v>
       </c>
       <c r="AL6">
-        <v>793419.0000000001</v>
+        <v>793419.00000000012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>